<commit_message>
Bug with info screen fixed
</commit_message>
<xml_diff>
--- a/BoxTask/data/ID_21.xlsx
+++ b/BoxTask/data/ID_21.xlsx
@@ -7,16 +7,50 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="block0_trial0" sheetId="1" r:id="rId1"/>
+    <sheet name="block1_trial1" sheetId="2" r:id="rId2"/>
+    <sheet name="block1_trial2" sheetId="3" r:id="rId3"/>
+    <sheet name="block1_trial3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+  <si>
+    <t>Box_Num</t>
+  </si>
+  <si>
+    <t>Probability_Estimates</t>
+  </si>
+  <si>
+    <t>Reaction_time</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +66,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +74,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +392,431 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1.189881000085734</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>2.210181599948555</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0.7636415000306442</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>1.571190999937244</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1.533641500049271</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1.262780299992301</v>
+      </c>
+      <c r="E2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>1.583964899997227</v>
+      </c>
+      <c r="E3">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1.004658200079575</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1.682831900077872</v>
+      </c>
+      <c r="E5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>1.522029899992049</v>
+      </c>
+      <c r="E6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1.250530199962668</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>1.743581000017002</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>0.648053599987179</v>
+      </c>
+      <c r="E9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>1.980043399962597</v>
+      </c>
+      <c r="E10">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>1.363771399948746</v>
+      </c>
+      <c r="E11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>1.487020000000484</v>
+      </c>
+      <c r="E12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>0.5932290999917313</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>-1</v>
+      </c>
+      <c r="D14">
+        <v>-1</v>
+      </c>
+      <c r="E14">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>